<commit_message>
Added Eagle Lake Thermocline post
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Pike_Chain_WQ_Data.xlsx
+++ b/portfolio/posts/_data/Pike_Chain_WQ_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="2" r:id="rId1"/>
@@ -18,12 +18,15 @@
     <sheet name="Comments" sheetId="5" r:id="rId4"/>
     <sheet name="Observer" sheetId="1" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DO!$A$1:$I$772</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9089" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9098" uniqueCount="477">
   <si>
     <t>Buskey Bay</t>
   </si>
@@ -1431,6 +1434,30 @@
   <si>
     <t>Updated all data from WiDNR website through 2022</t>
   </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Temp originally entered as 488.1</t>
+  </si>
+  <si>
+    <t>Temp originally entered as 0.07</t>
+  </si>
+  <si>
+    <t>Temp originally entered as 588.7</t>
+  </si>
+  <si>
+    <t>Temp originally entered as 49.88</t>
+  </si>
+  <si>
+    <t>DO originally entered as 88.97'</t>
+  </si>
+  <si>
+    <t>Is this Temp correct?</t>
+  </si>
+  <si>
+    <t>Temp was originally 49.3</t>
+  </si>
 </sst>
 </file>
 
@@ -23446,11 +23473,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H772"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:I772"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A671" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E684" sqref="E684"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23465,7 +23493,7 @@
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>73</v>
       </c>
@@ -23490,8 +23518,11 @@
       <c r="H1" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="3" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -23511,7 +23542,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -23531,7 +23562,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -23551,7 +23582,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -23571,7 +23602,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -23591,7 +23622,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -23611,7 +23642,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -23631,7 +23662,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -23651,7 +23682,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -23677,7 +23708,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>79</v>
       </c>
@@ -23703,7 +23734,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>79</v>
       </c>
@@ -23729,7 +23760,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>79</v>
       </c>
@@ -23755,7 +23786,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -23781,7 +23812,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>79</v>
       </c>
@@ -23807,7 +23838,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>79</v>
       </c>
@@ -28265,7 +28296,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>79</v>
       </c>
@@ -28291,7 +28322,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>79</v>
       </c>
@@ -28317,7 +28348,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>79</v>
       </c>
@@ -28343,7 +28374,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>79</v>
       </c>
@@ -28369,7 +28400,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>79</v>
       </c>
@@ -28395,7 +28426,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>79</v>
       </c>
@@ -28421,7 +28452,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>79</v>
       </c>
@@ -28447,7 +28478,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>79</v>
       </c>
@@ -28473,7 +28504,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>79</v>
       </c>
@@ -28499,7 +28530,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>79</v>
       </c>
@@ -28525,7 +28556,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>79</v>
       </c>
@@ -28551,7 +28582,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>79</v>
       </c>
@@ -28577,7 +28608,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>79</v>
       </c>
@@ -28603,7 +28634,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>79</v>
       </c>
@@ -28628,8 +28659,11 @@
       <c r="H206" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I206" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>79</v>
       </c>
@@ -28655,7 +28689,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>79</v>
       </c>
@@ -35479,7 +35513,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="476" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A476" t="s">
         <v>204</v>
       </c>
@@ -35499,7 +35533,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="477" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A477" t="s">
         <v>204</v>
       </c>
@@ -35519,7 +35553,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="478" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A478" t="s">
         <v>204</v>
       </c>
@@ -35539,7 +35573,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="479" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A479" t="s">
         <v>204</v>
       </c>
@@ -35559,7 +35593,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="480" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A480" t="s">
         <v>204</v>
       </c>
@@ -35579,7 +35613,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="481" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A481" t="s">
         <v>204</v>
       </c>
@@ -35599,7 +35633,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="482" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A482" t="s">
         <v>204</v>
       </c>
@@ -35613,7 +35647,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="483" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A483" t="s">
         <v>204</v>
       </c>
@@ -35627,7 +35661,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="484" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A484" t="s">
         <v>204</v>
       </c>
@@ -35641,7 +35675,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="485" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A485" t="s">
         <v>204</v>
       </c>
@@ -35655,7 +35689,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="486" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A486" t="s">
         <v>204</v>
       </c>
@@ -35669,7 +35703,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="487" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A487" t="s">
         <v>204</v>
       </c>
@@ -35683,7 +35717,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="488" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A488" t="s">
         <v>204</v>
       </c>
@@ -35697,7 +35731,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="489" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A489" t="s">
         <v>204</v>
       </c>
@@ -35711,7 +35745,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="490" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A490" t="s">
         <v>204</v>
       </c>
@@ -35725,7 +35759,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="491" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A491" t="s">
         <v>204</v>
       </c>
@@ -35739,7 +35773,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="492" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A492" t="s">
         <v>204</v>
       </c>
@@ -35753,7 +35787,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="493" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A493" t="s">
         <v>204</v>
       </c>
@@ -35779,7 +35813,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="494" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A494" t="s">
         <v>237</v>
       </c>
@@ -35799,7 +35833,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="495" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A495" t="s">
         <v>237</v>
       </c>
@@ -35819,7 +35853,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="496" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A496" t="s">
         <v>237</v>
       </c>
@@ -35839,7 +35873,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="497" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
         <v>237</v>
       </c>
@@ -35859,7 +35893,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="498" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A498" t="s">
         <v>237</v>
       </c>
@@ -35879,7 +35913,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="499" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A499" t="s">
         <v>237</v>
       </c>
@@ -35899,7 +35933,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="500" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A500" t="s">
         <v>237</v>
       </c>
@@ -35919,7 +35953,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="501" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A501" t="s">
         <v>237</v>
       </c>
@@ -35939,7 +35973,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="502" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="502" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A502" t="s">
         <v>237</v>
       </c>
@@ -35965,7 +35999,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="503" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A503" t="s">
         <v>237</v>
       </c>
@@ -35991,7 +36025,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="504" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="504" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A504" t="s">
         <v>237</v>
       </c>
@@ -36017,7 +36051,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="505" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="505" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A505" t="s">
         <v>237</v>
       </c>
@@ -36043,7 +36077,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="506" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="506" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A506" t="s">
         <v>237</v>
       </c>
@@ -36069,7 +36103,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="507" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="507" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A507" t="s">
         <v>237</v>
       </c>
@@ -36095,7 +36129,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="508" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="508" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A508" t="s">
         <v>237</v>
       </c>
@@ -36121,7 +36155,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="509" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="509" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A509" t="s">
         <v>237</v>
       </c>
@@ -36147,7 +36181,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="510" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="510" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A510" t="s">
         <v>237</v>
       </c>
@@ -36173,7 +36207,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="511" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A511" t="s">
         <v>237</v>
       </c>
@@ -36199,7 +36233,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="512" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="512" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A512" t="s">
         <v>237</v>
       </c>
@@ -36225,7 +36259,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="513" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="513" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A513" t="s">
         <v>237</v>
       </c>
@@ -36251,7 +36285,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="514" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="514" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A514" t="s">
         <v>237</v>
       </c>
@@ -36277,7 +36311,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="515" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="515" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A515" t="s">
         <v>237</v>
       </c>
@@ -36303,7 +36337,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="516" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="516" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A516" t="s">
         <v>237</v>
       </c>
@@ -36329,7 +36363,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="517" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="517" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A517" t="s">
         <v>237</v>
       </c>
@@ -36355,7 +36389,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="518" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="518" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A518" t="s">
         <v>237</v>
       </c>
@@ -36369,7 +36403,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="519" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="519" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A519" t="s">
         <v>237</v>
       </c>
@@ -36383,7 +36417,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="520" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="520" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A520" t="s">
         <v>237</v>
       </c>
@@ -36397,7 +36431,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="521" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="521" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A521" t="s">
         <v>237</v>
       </c>
@@ -36411,7 +36445,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="522" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="522" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A522" t="s">
         <v>237</v>
       </c>
@@ -36425,7 +36459,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="523" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="523" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A523" t="s">
         <v>237</v>
       </c>
@@ -36439,7 +36473,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="524" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="524" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A524" t="s">
         <v>237</v>
       </c>
@@ -36453,7 +36487,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="525" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="525" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A525" t="s">
         <v>237</v>
       </c>
@@ -36467,7 +36501,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="526" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="526" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A526" t="s">
         <v>263</v>
       </c>
@@ -36487,7 +36521,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="527" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="527" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A527" t="s">
         <v>263</v>
       </c>
@@ -36507,7 +36541,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="528" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="528" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A528" t="s">
         <v>263</v>
       </c>
@@ -36527,7 +36561,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="529" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="529" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A529" t="s">
         <v>263</v>
       </c>
@@ -36547,7 +36581,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="530" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="530" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A530" t="s">
         <v>263</v>
       </c>
@@ -36567,7 +36601,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="531" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="531" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A531" t="s">
         <v>263</v>
       </c>
@@ -36587,7 +36621,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="532" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="532" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A532" t="s">
         <v>298</v>
       </c>
@@ -36607,7 +36641,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="533" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="533" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A533" t="s">
         <v>298</v>
       </c>
@@ -36627,7 +36661,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="534" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="534" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A534" t="s">
         <v>298</v>
       </c>
@@ -36647,7 +36681,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="535" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="535" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A535" t="s">
         <v>298</v>
       </c>
@@ -36667,7 +36701,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="536" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="536" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A536" t="s">
         <v>298</v>
       </c>
@@ -36687,7 +36721,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="537" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="537" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A537" t="s">
         <v>298</v>
       </c>
@@ -36707,7 +36741,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="538" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="538" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A538" t="s">
         <v>298</v>
       </c>
@@ -36727,7 +36761,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="539" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="539" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A539" t="s">
         <v>298</v>
       </c>
@@ -36747,7 +36781,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="540" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="540" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A540" t="s">
         <v>298</v>
       </c>
@@ -36767,7 +36801,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="541" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="541" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A541" t="s">
         <v>298</v>
       </c>
@@ -36787,7 +36821,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="542" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="542" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A542" t="s">
         <v>298</v>
       </c>
@@ -36807,7 +36841,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="543" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="543" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A543" t="s">
         <v>298</v>
       </c>
@@ -36827,7 +36861,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="544" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="544" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A544" t="s">
         <v>298</v>
       </c>
@@ -36847,7 +36881,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="545" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="545" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A545" t="s">
         <v>298</v>
       </c>
@@ -36867,7 +36901,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="546" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="546" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A546" t="s">
         <v>298</v>
       </c>
@@ -36887,7 +36921,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="547" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="547" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A547" t="s">
         <v>298</v>
       </c>
@@ -36907,7 +36941,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="548" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="548" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A548" t="s">
         <v>298</v>
       </c>
@@ -36927,7 +36961,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="549" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="549" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A549" t="s">
         <v>298</v>
       </c>
@@ -36947,7 +36981,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="550" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="550" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A550" t="s">
         <v>298</v>
       </c>
@@ -36967,7 +37001,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="551" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="551" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A551" t="s">
         <v>298</v>
       </c>
@@ -36987,7 +37021,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="552" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="552" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A552" t="s">
         <v>298</v>
       </c>
@@ -37007,7 +37041,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="553" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="553" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A553" t="s">
         <v>298</v>
       </c>
@@ -37027,7 +37061,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="554" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="554" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A554" t="s">
         <v>298</v>
       </c>
@@ -37047,7 +37081,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="555" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="555" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A555" t="s">
         <v>298</v>
       </c>
@@ -37067,7 +37101,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="556" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="556" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A556" t="s">
         <v>298</v>
       </c>
@@ -37087,7 +37121,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="557" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="557" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A557" t="s">
         <v>298</v>
       </c>
@@ -37185,7 +37219,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="561" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="561" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A561" t="s">
         <v>79</v>
       </c>
@@ -37211,7 +37245,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="562" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="562" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A562" t="s">
         <v>79</v>
       </c>
@@ -37237,7 +37271,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="563" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="563" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A563" t="s">
         <v>79</v>
       </c>
@@ -37263,7 +37297,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="564" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="564" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A564" t="s">
         <v>79</v>
       </c>
@@ -37289,7 +37323,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="565" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="565" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A565" t="s">
         <v>79</v>
       </c>
@@ -37315,7 +37349,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="566" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="566" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A566" t="s">
         <v>79</v>
       </c>
@@ -37341,7 +37375,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="567" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="567" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A567" t="s">
         <v>79</v>
       </c>
@@ -37367,7 +37401,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="568" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="568" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A568" t="s">
         <v>79</v>
       </c>
@@ -37393,7 +37427,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="569" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="569" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A569" t="s">
         <v>79</v>
       </c>
@@ -37419,7 +37453,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="570" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="570" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A570" t="s">
         <v>79</v>
       </c>
@@ -37445,7 +37479,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="571" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="571" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A571" t="s">
         <v>79</v>
       </c>
@@ -37471,7 +37505,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="572" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="572" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A572" t="s">
         <v>79</v>
       </c>
@@ -37497,7 +37531,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="573" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="573" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A573" t="s">
         <v>79</v>
       </c>
@@ -37523,7 +37557,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="574" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="574" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A574" t="s">
         <v>79</v>
       </c>
@@ -37549,7 +37583,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="575" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="575" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A575" t="s">
         <v>79</v>
       </c>
@@ -37575,7 +37609,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="576" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="576" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A576" t="s">
         <v>79</v>
       </c>
@@ -37589,7 +37623,7 @@
         <v>80</v>
       </c>
       <c r="E576">
-        <v>488.1</v>
+        <v>48.1</v>
       </c>
       <c r="F576" t="s">
         <v>81</v>
@@ -37600,8 +37634,11 @@
       <c r="H576" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="577" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I576" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="577" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A577" t="s">
         <v>79</v>
       </c>
@@ -37627,7 +37664,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="578" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="578" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A578" t="s">
         <v>79</v>
       </c>
@@ -37653,7 +37690,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="579" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="579" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A579" t="s">
         <v>79</v>
       </c>
@@ -37666,14 +37703,14 @@
       <c r="D579" t="s">
         <v>80</v>
       </c>
-      <c r="E579">
-        <v>7.0000000000000007E-2</v>
-      </c>
       <c r="F579" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="580" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I579" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="580" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A580" t="s">
         <v>79</v>
       </c>
@@ -37699,7 +37736,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="581" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="581" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A581" t="s">
         <v>79</v>
       </c>
@@ -37725,7 +37762,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="582" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="582" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A582" t="s">
         <v>79</v>
       </c>
@@ -37751,7 +37788,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="583" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="583" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A583" t="s">
         <v>79</v>
       </c>
@@ -37777,7 +37814,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="584" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="584" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A584" t="s">
         <v>79</v>
       </c>
@@ -37803,7 +37840,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="585" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="585" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A585" t="s">
         <v>79</v>
       </c>
@@ -37829,7 +37866,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="586" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="586" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A586" t="s">
         <v>79</v>
       </c>
@@ -37849,13 +37886,16 @@
         <v>81</v>
       </c>
       <c r="G586">
-        <v>88.97</v>
+        <v>8.9700000000000006</v>
       </c>
       <c r="H586" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="587" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I586" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="587" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A587" t="s">
         <v>79</v>
       </c>
@@ -37881,7 +37921,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="588" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="588" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A588" t="s">
         <v>79</v>
       </c>
@@ -37907,7 +37947,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="589" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="589" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A589" t="s">
         <v>79</v>
       </c>
@@ -37933,7 +37973,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="590" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="590" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A590" t="s">
         <v>79</v>
       </c>
@@ -37947,7 +37987,7 @@
         <v>80</v>
       </c>
       <c r="E590">
-        <v>588.70000000000005</v>
+        <v>58.7</v>
       </c>
       <c r="F590" t="s">
         <v>81</v>
@@ -37958,8 +37998,11 @@
       <c r="H590" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="591" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I590" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="591" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A591" t="s">
         <v>79</v>
       </c>
@@ -37985,7 +38028,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="592" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="592" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A592" t="s">
         <v>79</v>
       </c>
@@ -38011,7 +38054,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="593" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="593" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A593" t="s">
         <v>79</v>
       </c>
@@ -38025,7 +38068,7 @@
         <v>80</v>
       </c>
       <c r="E593">
-        <v>49.88</v>
+        <v>49.8</v>
       </c>
       <c r="F593" t="s">
         <v>81</v>
@@ -38036,8 +38079,11 @@
       <c r="H593" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="594" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I593" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="594" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A594" t="s">
         <v>79</v>
       </c>
@@ -38063,7 +38109,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="595" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="595" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A595" t="s">
         <v>79</v>
       </c>
@@ -38089,7 +38135,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="596" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="596" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A596" t="s">
         <v>79</v>
       </c>
@@ -38115,7 +38161,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="597" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="597" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A597" t="s">
         <v>79</v>
       </c>
@@ -38141,7 +38187,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="598" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="598" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A598" t="s">
         <v>79</v>
       </c>
@@ -38167,7 +38213,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="599" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="599" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A599" t="s">
         <v>79</v>
       </c>
@@ -38193,7 +38239,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="600" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="600" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A600" t="s">
         <v>79</v>
       </c>
@@ -38219,7 +38265,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="601" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="601" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A601" t="s">
         <v>79</v>
       </c>
@@ -38245,7 +38291,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="602" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="602" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A602" t="s">
         <v>79</v>
       </c>
@@ -38271,7 +38317,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="603" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="603" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A603" t="s">
         <v>79</v>
       </c>
@@ -38297,7 +38343,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="604" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="604" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A604" t="s">
         <v>79</v>
       </c>
@@ -38323,7 +38369,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="605" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="605" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A605" t="s">
         <v>79</v>
       </c>
@@ -38349,7 +38395,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="606" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="606" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A606" t="s">
         <v>79</v>
       </c>
@@ -38375,7 +38421,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="607" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="607" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A607" t="s">
         <v>79</v>
       </c>
@@ -38401,7 +38447,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="608" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="608" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A608" t="s">
         <v>79</v>
       </c>
@@ -38415,7 +38461,7 @@
         <v>80</v>
       </c>
       <c r="E608">
-        <v>488.1</v>
+        <v>48.1</v>
       </c>
       <c r="F608" t="s">
         <v>81</v>
@@ -38426,6 +38472,9 @@
       <c r="H608" t="s">
         <v>35</v>
       </c>
+      <c r="I608" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="609" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A609" t="s">
@@ -40091,7 +40140,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="673" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="673" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A673" t="s">
         <v>79</v>
       </c>
@@ -40117,7 +40166,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="674" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="674" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A674" t="s">
         <v>79</v>
       </c>
@@ -40143,7 +40192,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="675" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="675" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A675" t="s">
         <v>79</v>
       </c>
@@ -40169,7 +40218,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="676" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="676" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A676" t="s">
         <v>79</v>
       </c>
@@ -40195,7 +40244,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="677" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="677" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A677" t="s">
         <v>79</v>
       </c>
@@ -40221,7 +40270,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="678" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="678" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A678" t="s">
         <v>79</v>
       </c>
@@ -40247,7 +40296,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="679" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="679" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A679" t="s">
         <v>79</v>
       </c>
@@ -40273,7 +40322,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="680" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="680" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A680" t="s">
         <v>79</v>
       </c>
@@ -40299,7 +40348,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="681" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="681" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A681" t="s">
         <v>79</v>
       </c>
@@ -40325,7 +40374,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="682" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="682" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A682" t="s">
         <v>79</v>
       </c>
@@ -40351,7 +40400,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="683" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="683" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A683" t="s">
         <v>79</v>
       </c>
@@ -40365,7 +40414,7 @@
         <v>80</v>
       </c>
       <c r="E683">
-        <v>49.3</v>
+        <v>44.3</v>
       </c>
       <c r="F683" t="s">
         <v>81</v>
@@ -40376,8 +40425,11 @@
       <c r="H683" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="684" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I683" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="684" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A684" t="s">
         <v>79</v>
       </c>
@@ -40403,7 +40455,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="685" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="685" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A685" t="s">
         <v>79</v>
       </c>
@@ -40429,7 +40481,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="686" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="686" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A686" t="s">
         <v>79</v>
       </c>
@@ -40455,7 +40507,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="687" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="687" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A687" t="s">
         <v>79</v>
       </c>
@@ -40481,7 +40533,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="688" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="688" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A688" t="s">
         <v>79</v>
       </c>
@@ -42509,7 +42561,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="766" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="766" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A766" t="s">
         <v>204</v>
       </c>
@@ -42535,7 +42587,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="767" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="767" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A767" t="s">
         <v>204</v>
       </c>
@@ -42561,7 +42613,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="768" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="768" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A768" t="s">
         <v>204</v>
       </c>
@@ -42587,7 +42639,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="769" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="769" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A769" t="s">
         <v>204</v>
       </c>
@@ -42613,7 +42665,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="770" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="770" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A770" t="s">
         <v>204</v>
       </c>
@@ -42639,7 +42691,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="771" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="771" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A771" t="s">
         <v>204</v>
       </c>
@@ -42665,7 +42717,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="772" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="772" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A772" t="s">
         <v>204</v>
       </c>
@@ -42692,6 +42744,16 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I772">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Eagle Lake"/>
+      </filters>
+    </filterColumn>
+    <sortState ref="A10:I765">
+      <sortCondition ref="B1:B772"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -47294,9 +47356,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D632"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D629" sqref="D629"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>